<commit_message>
Changed column order in Instruments tab in test_excel_ui.py.
</commit_message>
<xml_diff>
--- a/test/test_excel_ui.xlsx
+++ b/test/test_excel_ui.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -545,8 +545,8 @@
     <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -563,10 +563,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -583,10 +583,10 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -603,10 +603,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -747,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>